<commit_message>
Complete the 50 problems
</commit_message>
<xml_diff>
--- a/SDE 2026 - Rating.xlsx
+++ b/SDE 2026 - Rating.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\academics\New_folder\competitive programng\50-days challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DAA81-6441-403D-92AC-2EC1567A8FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF5513D-5B8A-4BBC-AF74-12746F62B5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="116">
   <si>
     <t>S.No</t>
   </si>
@@ -371,6 +371,18 @@
   </si>
   <si>
     <t>O(nlogn)</t>
+  </si>
+  <si>
+    <t>O(N!)</t>
+  </si>
+  <si>
+    <t>sliding window + hashing</t>
+  </si>
+  <si>
+    <t>O(k+n)</t>
+  </si>
+  <si>
+    <t>binary search + 2d dynamic programming</t>
   </si>
 </sst>
 </file>
@@ -463,12 +475,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -704,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -739,1020 +750,1038 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7">
+    <row r="2" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7">
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7">
+    <row r="4" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="D6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="D7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7">
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="D9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7">
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7">
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="D11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="7">
+    <row r="12" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="7">
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="D13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="7">
+    <row r="14" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="D14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="7">
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="7">
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="C16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7">
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="7">
+    <row r="18" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="C18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="7">
+    <row r="19" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="C19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="7">
+    <row r="20" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="C20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="8" t="s">
+      <c r="C21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="7">
+    <row r="22" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
-      <c r="A23" s="7">
+    <row r="23" spans="1:6" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="C23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="7">
+    <row r="24" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="C24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="7">
+    <row r="25" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="C25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="7">
+    <row r="26" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="C26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="7">
+    <row r="27" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="8" t="s">
+      <c r="C27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="7">
+    <row r="28" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="C28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="7">
+    <row r="29" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="C29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="7">
+    <row r="30" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="C30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="7">
+    <row r="31" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="C31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="7">
+    <row r="32" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="8" t="s">
+      <c r="C32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="7">
+    <row r="33" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="8" t="s">
+      <c r="C33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="7">
+    <row r="34" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="6">
         <v>33</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="7">
+    <row r="35" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="6">
         <v>34</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="8" t="s">
+      <c r="C35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="7">
+    <row r="36" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="8" t="s">
+      <c r="C36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="7">
+    <row r="37" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="6">
         <v>36</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="8" t="s">
+      <c r="C37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="7">
+    <row r="38" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="6">
         <v>37</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="8" t="s">
+      <c r="C38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F38" s="8" t="s">
+      <c r="E38" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="7">
+    <row r="39" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="6">
         <v>38</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="8" t="s">
+      <c r="C39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="7">
+    <row r="40" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="6">
         <v>39</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="C40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="7">
+    <row r="41" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="8" t="s">
+      <c r="C41" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="7">
+    <row r="42" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="6">
         <v>41</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="8" t="s">
+      <c r="C42" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="11">
+    <row r="43" spans="1:6" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="10">
         <v>42</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="12" t="s">
+      <c r="C43" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F43" s="13" t="s">
+      <c r="F43" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
-      <c r="A44" s="7">
+    <row r="44" spans="1:6" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A44" s="6">
         <v>43</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="7">
+    <row r="45" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="6">
         <v>44</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="7">
+    <row r="46" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" s="8" t="s">
+      <c r="D46" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="7">
+    <row r="47" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="6">
         <v>46</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="7">
+    <row r="48" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="6">
         <v>47</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="4">
+    <row r="49" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="6">
         <v>48</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="4">
+      <c r="D49" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="6">
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="4">
+      <c r="D50" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="6">
         <v>50</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
+      <c r="D51" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F52" s="5"/>
+      <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="5" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>